<commit_message>
Finished individual category analysis. TODO: Pivot analysis
</commit_message>
<xml_diff>
--- a/task/ColumnAnalysis.xlsx
+++ b/task/ColumnAnalysis.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\DemayDemographics\task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958AFF50-B347-4341-8E34-DC1DD33B1D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80678B0C-1634-45EF-8565-243BF660BE77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16416" yWindow="0" windowWidth="16416" windowHeight="21432" xr2:uid="{2BFD14B1-31E7-40E5-A2EA-3DA81C19F690}"/>
   </bookViews>
   <sheets>
-    <sheet name="names" sheetId="1" r:id="rId1"/>
-    <sheet name="patterns" sheetId="2" r:id="rId2"/>
+    <sheet name="schema" sheetId="3" r:id="rId1"/>
+    <sheet name="names" sheetId="1" r:id="rId2"/>
+    <sheet name="patterns" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="195">
   <si>
     <t>ii. Date (yyyy)</t>
   </si>
@@ -467,6 +468,150 @@
   </si>
   <si>
     <t>Dphil</t>
+  </si>
+  <si>
+    <t>'1. Sex assigned at birth': 'string',</t>
+  </si>
+  <si>
+    <t>2. Gender Identity': 'string',</t>
+  </si>
+  <si>
+    <t>Black or African American': 'string',</t>
+  </si>
+  <si>
+    <t>Hispanic or Latino': 'string',</t>
+  </si>
+  <si>
+    <t>American Indian or Alaskan Native': 'string',</t>
+  </si>
+  <si>
+    <t>Native Hawaiian and other Pacific Islander': 'string',</t>
+  </si>
+  <si>
+    <t>Cambodian or Laotian': 'string',</t>
+  </si>
+  <si>
+    <t>None': 'string',</t>
+  </si>
+  <si>
+    <t>Prefer not to answer': 'string',</t>
+  </si>
+  <si>
+    <t>4. Identification as ': 'string',</t>
+  </si>
+  <si>
+    <t>5. Requirement for workplace accommodations: (Reasonable accommodations in the workplace support people with disability and/or chronic health conditions in performing their jobs.) If you would like more information about obtaining accommodations, contact MGH OHS.': 'string',</t>
+  </si>
+  <si>
+    <t>1. Are you considering or engaging in the process of retirement? ': 'string',</t>
+  </si>
+  <si>
+    <t>2. Are you interested in learning more about HMS promotions and discussing advancement on the HMS ladder? ': 'string',</t>
+  </si>
+  <si>
+    <t>MD': 'string',</t>
+  </si>
+  <si>
+    <t>MBChB': 'string',</t>
+  </si>
+  <si>
+    <t>DO': 'string',</t>
+  </si>
+  <si>
+    <t>PhD': 'string',</t>
+  </si>
+  <si>
+    <t>DPhil': 'string',</t>
+  </si>
+  <si>
+    <t>Sci D': 'string',</t>
+  </si>
+  <si>
+    <t>RDN': 'string',</t>
+  </si>
+  <si>
+    <t>MS': 'string',</t>
+  </si>
+  <si>
+    <t>MSN': 'string',</t>
+  </si>
+  <si>
+    <t>MPH': 'string',</t>
+  </si>
+  <si>
+    <t>MPA': 'string',</t>
+  </si>
+  <si>
+    <t>MBA': 'string',</t>
+  </si>
+  <si>
+    <t>Other': 'string',</t>
+  </si>
+  <si>
+    <t>i. HMS Rank': 'string',</t>
+  </si>
+  <si>
+    <t>ii. Date (yyyy)': 'string',</t>
+  </si>
+  <si>
+    <t>i. HMS Rank.1': 'string',</t>
+  </si>
+  <si>
+    <t>ii. Date (yyyy).1': 'string',</t>
+  </si>
+  <si>
+    <t>i. HMS Rank.2': 'string',</t>
+  </si>
+  <si>
+    <t>ii. Date (yyyy).2': 'string',</t>
+  </si>
+  <si>
+    <t>i. HMS Rank.3': 'string',</t>
+  </si>
+  <si>
+    <t>ii. Date (yyyy).3': 'string',</t>
+  </si>
+  <si>
+    <t>i. HMS Rank.4': 'string',</t>
+  </si>
+  <si>
+    <t>ii. Date (yyyy).4': 'string',</t>
+  </si>
+  <si>
+    <t>i. Job Title': 'string',</t>
+  </si>
+  <si>
+    <t>ii. Date (yyyy).5': 'string',</t>
+  </si>
+  <si>
+    <t>i. Job Title.1': 'string',</t>
+  </si>
+  <si>
+    <t>ii. Date (yyyy).6': 'string',</t>
+  </si>
+  <si>
+    <t>i. Job Title.2': 'string',</t>
+  </si>
+  <si>
+    <t>ii. Date (yyyy).7': 'string',</t>
+  </si>
+  <si>
+    <t>i. Job Title.3': 'string',</t>
+  </si>
+  <si>
+    <t>ii. Date (yyyy).8': 'string',</t>
+  </si>
+  <si>
+    <t>i. Job Title.4': 'string',</t>
+  </si>
+  <si>
+    <t>ii. Date (yyyy).9': 'string',</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Descr</t>
   </si>
 </sst>
 </file>
@@ -550,7 +695,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -558,6 +703,10 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -872,11 +1021,405 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F26F13AB-4F43-4B31-98C5-AF1A4D6CDCA0}">
+  <dimension ref="B1:C47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="5.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="8">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="8">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="8">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="8">
+        <v>3</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" s="8">
+        <v>4</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B7" s="8">
+        <v>5</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="8">
+        <v>6</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B9" s="8">
+        <v>7</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="8">
+        <v>8</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="8">
+        <v>9</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B12" s="8">
+        <v>10</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B13" s="8">
+        <v>11</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B14" s="8">
+        <v>12</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B15" s="8">
+        <v>13</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B16" s="8">
+        <v>14</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="8">
+        <v>15</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="8">
+        <v>16</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="8">
+        <v>17</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="8">
+        <v>18</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" s="8">
+        <v>19</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" s="8">
+        <v>20</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23" s="8">
+        <v>21</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24" s="8">
+        <v>22</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B25" s="8">
+        <v>23</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B26" s="8">
+        <v>24</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B27" s="8">
+        <v>25</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B28" s="8">
+        <v>26</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B29" s="8">
+        <v>27</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B30" s="8">
+        <v>28</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B31" s="8">
+        <v>29</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B32" s="8">
+        <v>30</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B33" s="8">
+        <v>31</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B34" s="8">
+        <v>32</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B35" s="8">
+        <v>33</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B36" s="8">
+        <v>34</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B37" s="8">
+        <v>35</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B38" s="8">
+        <v>36</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B39" s="8">
+        <v>37</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B40" s="8">
+        <v>38</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B41" s="8">
+        <v>39</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B42" s="8">
+        <v>40</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B43" s="8">
+        <v>41</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B44" s="8">
+        <v>42</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B45" s="8">
+        <v>43</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B46" s="8">
+        <v>44</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B47" s="8">
+        <v>45</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>192</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A1E9517-2074-4D0D-9DBC-DCDC92671B7E}">
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2056,7 +2599,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9FC61BD-9B33-4288-85CD-7ECB340DABDF}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>

<commit_message>
HMSPromo analysis up to URIM cross tabulation
</commit_message>
<xml_diff>
--- a/task/ColumnAnalysis.xlsx
+++ b/task/ColumnAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\DemayDemographics\task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80678B0C-1634-45EF-8565-243BF660BE77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{507B43E3-1453-496E-9BAA-F58DBC159CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16416" yWindow="0" windowWidth="16416" windowHeight="21432" xr2:uid="{2BFD14B1-31E7-40E5-A2EA-3DA81C19F690}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="200">
   <si>
     <t>ii. Date (yyyy)</t>
   </si>
@@ -497,12 +497,6 @@
     <t>Prefer not to answer': 'string',</t>
   </si>
   <si>
-    <t>4. Identification as ': 'string',</t>
-  </si>
-  <si>
-    <t>5. Requirement for workplace accommodations: (Reasonable accommodations in the workplace support people with disability and/or chronic health conditions in performing their jobs.) If you would like more information about obtaining accommodations, contact MGH OHS.': 'string',</t>
-  </si>
-  <si>
     <t>1. Are you considering or engaging in the process of retirement? ': 'string',</t>
   </si>
   <si>
@@ -612,6 +606,27 @@
   </si>
   <si>
     <t>Descr</t>
+  </si>
+  <si>
+    <t>Orientation: 'string',</t>
+  </si>
+  <si>
+    <t>Accomodations: 'string',</t>
+  </si>
+  <si>
+    <t>urmNoAnswer</t>
+  </si>
+  <si>
+    <t>degClinical</t>
+  </si>
+  <si>
+    <t>degNonClinical</t>
+  </si>
+  <si>
+    <t>degOther</t>
+  </si>
+  <si>
+    <t>degNoAnswer</t>
   </si>
 </sst>
 </file>
@@ -1022,10 +1037,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F26F13AB-4F43-4B31-98C5-AF1A4D6CDCA0}">
-  <dimension ref="B1:C47"/>
+  <dimension ref="B1:C52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1035,10 +1050,10 @@
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
@@ -1118,7 +1133,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>156</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.3">
@@ -1126,7 +1141,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>157</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.3">
@@ -1134,7 +1149,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.3">
@@ -1142,7 +1157,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.3">
@@ -1150,7 +1165,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.3">
@@ -1158,7 +1173,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
@@ -1166,7 +1181,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
@@ -1174,7 +1189,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.3">
@@ -1182,7 +1197,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.3">
@@ -1190,7 +1205,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.3">
@@ -1198,7 +1213,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.3">
@@ -1206,7 +1221,7 @@
         <v>20</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.3">
@@ -1214,7 +1229,7 @@
         <v>21</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.3">
@@ -1222,7 +1237,7 @@
         <v>22</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.3">
@@ -1230,7 +1245,7 @@
         <v>23</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.3">
@@ -1238,7 +1253,7 @@
         <v>24</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.3">
@@ -1246,7 +1261,7 @@
         <v>25</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.3">
@@ -1254,7 +1269,7 @@
         <v>26</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.3">
@@ -1262,7 +1277,7 @@
         <v>27</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.3">
@@ -1270,7 +1285,7 @@
         <v>28</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.3">
@@ -1278,7 +1293,7 @@
         <v>29</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.3">
@@ -1286,7 +1301,7 @@
         <v>30</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.3">
@@ -1294,7 +1309,7 @@
         <v>31</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.3">
@@ -1302,7 +1317,7 @@
         <v>32</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.3">
@@ -1310,7 +1325,7 @@
         <v>33</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.3">
@@ -1318,7 +1333,7 @@
         <v>34</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.3">
@@ -1326,7 +1341,7 @@
         <v>35</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.3">
@@ -1334,7 +1349,7 @@
         <v>36</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.3">
@@ -1342,7 +1357,7 @@
         <v>37</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.3">
@@ -1350,7 +1365,7 @@
         <v>38</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.3">
@@ -1358,7 +1373,7 @@
         <v>39</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.3">
@@ -1366,7 +1381,7 @@
         <v>40</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.3">
@@ -1374,7 +1389,7 @@
         <v>41</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.3">
@@ -1382,7 +1397,7 @@
         <v>42</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.3">
@@ -1390,7 +1405,7 @@
         <v>43</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.3">
@@ -1398,7 +1413,7 @@
         <v>44</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.3">
@@ -1406,7 +1421,47 @@
         <v>45</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B48" s="8">
+        <v>-5</v>
+      </c>
+      <c r="C48" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B49" s="8">
+        <v>-4</v>
+      </c>
+      <c r="C49" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B50" s="8">
+        <v>-3</v>
+      </c>
+      <c r="C50" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B51" s="8">
+        <v>-2</v>
+      </c>
+      <c r="C51" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B52" s="8">
+        <v>-1</v>
+      </c>
+      <c r="C52" t="s">
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>